<commit_message>
Fixing the executable jar file
</commit_message>
<xml_diff>
--- a/examples/results/T002a/T002_0_0.xlsx
+++ b/examples/results/T002a/T002_0_0.xlsx
@@ -6,13 +6,16 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet0" r:id="rId3" sheetId="1"/>
+    <sheet name="CANONICAL TABLE" r:id="rId3" sheetId="1"/>
+    <sheet name="ENTRIES" r:id="rId4" sheetId="2"/>
+    <sheet name="LABELS" r:id="rId5" sheetId="3"/>
+    <sheet name="INFO" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="41">
   <si>
     <t>DATA</t>
   </si>
@@ -32,30 +35,30 @@
     <t>2</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
     <t>f</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
     <t>c</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
@@ -78,6 +81,63 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>ENTRY</t>
+  </si>
+  <si>
+    <t>PROVENANCE</t>
+  </si>
+  <si>
+    <t>LABELS</t>
+  </si>
+  <si>
+    <t>"b [F2]", "g [B4]", "i [C4]", "f [G3]"</t>
+  </si>
+  <si>
+    <t>"a [D2]", "g [B4]", "j [C5]", "c [D3]"</t>
+  </si>
+  <si>
+    <t>"a [D2]", "h [B6]", "k [C6]", "c [D3]"</t>
+  </si>
+  <si>
+    <t>"b [F2]", "g [B4]", "j [C5]", "f [G3]"</t>
+  </si>
+  <si>
+    <t>"b [F2]", "h [B6]", "k [C6]", "f [G3]"</t>
+  </si>
+  <si>
+    <t>"a [D2]", "g [B4]", "j [C5]", "d [E3]"</t>
+  </si>
+  <si>
+    <t>"a [D2]", "h [B6]", "k [C6]", "d [E3]"</t>
+  </si>
+  <si>
+    <t>"b [F2]", "g [B4]", "j [C5]", "e [F3]"</t>
+  </si>
+  <si>
+    <t>"b [F2]", "h [B6]", "k [C6]", "e [F3]"</t>
+  </si>
+  <si>
+    <t>"a [D2]", "g [B4]", "i [C4]", "c [D3]"</t>
+  </si>
+  <si>
+    <t>"a [D2]", "g [B4]", "i [C4]", "d [E3]"</t>
+  </si>
+  <si>
+    <t>"b [F2]", "g [B4]", "i [C4]", "e [F3]"</t>
+  </si>
+  <si>
+    <t>LABEL</t>
+  </si>
+  <si>
+    <t>PARENT</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>LINK TO THE SOURCE TABLE</t>
   </si>
 </sst>
 </file>
@@ -127,6 +187,13 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="5.82421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="8.640625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.640625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.640625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="8.640625" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -170,10 +237,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -187,13 +254,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -207,10 +274,10 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
@@ -221,13 +288,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -235,16 +302,16 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -252,16 +319,16 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -269,16 +336,16 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -286,16 +353,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -306,13 +373,13 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -320,16 +387,16 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
@@ -337,7 +404,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -346,7 +413,346 @@
         <v>8</v>
       </c>
       <c r="E13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="6.68359375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.3203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="32.14453125" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!G4","G4")</f>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!D5","D5")</f>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!D6","D6")</f>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!G5","G5")</f>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!G5","G5")</f>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!E5","E5")</f>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!E5","E5")</f>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!E5","E5")</f>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!E5","E5")</f>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!D4","D4")</f>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!D4","D4")</f>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!D4","D4")</f>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="6.24609375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.3203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.0234375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.63671875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!D2","D2")</f>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!F2","F2")</f>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!D3","D3")</f>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!E3","E3")</f>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!F3","F3")</f>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
         <v>9</v>
+      </c>
+      <c r="B7">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!G3","G3")</f>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!B4","B4")</f>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!C4","C4")</f>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!C5","C5")</f>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!B6","B6")</f>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!C6","C6")</f>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="25.7890625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1">
+        <f>HYPERLINK("[..\..\T002.xlsx]001!B2","[..\..\T002.xlsx]001!B2")</f>
       </c>
     </row>
   </sheetData>

</xml_diff>